<commit_message>
Alterações ref a Pendências de Validação v3.xlsx Adicionado nova versão bos Cadastrar Pesquisa-7.4.4.bos
</commit_message>
<xml_diff>
--- a/bos/Pendências de Validação v3.xlsx
+++ b/bos/Pendências de Validação v3.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emerson Aredes\Documents\GitHub\bonita-custom\bos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="11475" windowHeight="4620"/>
   </bookViews>
@@ -19,12 +14,46 @@
     <sheet name="PAIP" sheetId="4" r:id="rId5"/>
     <sheet name="Comprar Poster" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>gustavo</author>
+  </authors>
+  <commentList>
+    <comment ref="E111" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>gustavo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Script complexto, não dá tempo, precisa definir também se será usado máscara pro usuário inserir data manualmente, ou se usará um seletor de data... </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="304">
   <si>
     <t>Campo</t>
   </si>
@@ -949,12 +978,21 @@
   <si>
     <t>Se "utiliza material biológico" marcado como SIM, exibe os campos até Solicitar serviços</t>
   </si>
+  <si>
+    <t>Já estava feito</t>
+  </si>
+  <si>
+    <t>Não existe estilo justificado para campos de texto, nenhum navegador suporta</t>
+  </si>
+  <si>
+    <t>Complexo, tempo insuficiente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -976,6 +1014,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1016,7 +1067,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1052,6 +1103,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1061,16 +1116,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1131,7 +1201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1163,10 +1233,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1198,7 +1267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1374,27 +1442,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E130"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113:D119"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="109.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+    <row r="3" spans="1:4">
+      <c r="A3" s="19">
         <v>41565</v>
       </c>
       <c r="B3" t="s">
@@ -1407,8 +1476,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+    <row r="4" spans="1:4">
+      <c r="A4" s="20"/>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1419,8 +1488,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+    <row r="5" spans="1:4">
+      <c r="A5" s="20"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1431,8 +1500,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+    <row r="6" spans="1:4">
+      <c r="A6" s="20"/>
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -1440,8 +1509,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+    <row r="7" spans="1:4">
+      <c r="A7" s="20"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -1449,8 +1518,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:4">
+      <c r="A8" s="20"/>
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -1458,8 +1527,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+    <row r="9" spans="1:4">
+      <c r="A9" s="20"/>
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -1470,14 +1539,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+    <row r="10" spans="1:4">
+      <c r="A10" s="20"/>
       <c r="C10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+    <row r="11" spans="1:4">
+      <c r="A11" s="20"/>
       <c r="C11" t="s">
         <v>13</v>
       </c>
@@ -1485,8 +1554,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+    <row r="12" spans="1:4">
+      <c r="A12" s="20"/>
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -1497,8 +1566,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+    <row r="13" spans="1:4">
+      <c r="A13" s="20"/>
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1509,8 +1578,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+    <row r="14" spans="1:4">
+      <c r="A14" s="20"/>
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -1521,8 +1590,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+    <row r="15" spans="1:4">
+      <c r="A15" s="20"/>
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -1533,8 +1602,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+    <row r="16" spans="1:4">
+      <c r="A16" s="20"/>
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -1545,8 +1614,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+    <row r="17" spans="1:5">
+      <c r="A17" s="20"/>
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -1557,8 +1626,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+    <row r="18" spans="1:5">
+      <c r="A18" s="20"/>
       <c r="B18" t="s">
         <v>26</v>
       </c>
@@ -1572,8 +1641,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:5">
+      <c r="A19" s="20"/>
       <c r="B19" t="s">
         <v>27</v>
       </c>
@@ -1587,8 +1656,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+    <row r="20" spans="1:5">
+      <c r="A20" s="20"/>
       <c r="B20" t="s">
         <v>29</v>
       </c>
@@ -1599,8 +1668,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+    <row r="21" spans="1:5">
+      <c r="A21" s="20"/>
       <c r="C21" t="s">
         <v>31</v>
       </c>
@@ -1608,8 +1677,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+    <row r="22" spans="1:5">
+      <c r="A22" s="20"/>
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -1620,8 +1689,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+    <row r="23" spans="1:5">
+      <c r="A23" s="20"/>
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -1632,8 +1701,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+    <row r="24" spans="1:5">
+      <c r="A24" s="20"/>
       <c r="B24" t="s">
         <v>36</v>
       </c>
@@ -1644,8 +1713,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+    <row r="25" spans="1:5">
+      <c r="A25" s="20"/>
       <c r="B25" t="s">
         <v>50</v>
       </c>
@@ -1656,8 +1725,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+    <row r="26" spans="1:5">
+      <c r="A26" s="20"/>
       <c r="B26" t="s">
         <v>52</v>
       </c>
@@ -1668,8 +1737,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+    <row r="27" spans="1:5">
+      <c r="A27" s="20"/>
       <c r="B27" t="s">
         <v>54</v>
       </c>
@@ -1680,8 +1749,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+    <row r="28" spans="1:5">
+      <c r="A28" s="20"/>
       <c r="B28" t="s">
         <v>38</v>
       </c>
@@ -1692,8 +1761,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+    <row r="29" spans="1:5">
+      <c r="A29" s="20"/>
       <c r="C29" t="s">
         <v>40</v>
       </c>
@@ -1701,8 +1770,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+    <row r="30" spans="1:5">
+      <c r="A30" s="20"/>
       <c r="C30" t="s">
         <v>41</v>
       </c>
@@ -1710,8 +1779,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+    <row r="31" spans="1:5">
+      <c r="A31" s="20"/>
       <c r="C31" t="s">
         <v>42</v>
       </c>
@@ -1719,8 +1788,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+    <row r="32" spans="1:5">
+      <c r="A32" s="20"/>
       <c r="B32" t="s">
         <v>43</v>
       </c>
@@ -1728,8 +1797,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
+    <row r="33" spans="1:5">
+      <c r="A33" s="20"/>
       <c r="B33" t="s">
         <v>45</v>
       </c>
@@ -1737,8 +1806,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+    <row r="34" spans="1:5">
+      <c r="A34" s="20"/>
       <c r="B34" t="s">
         <v>47</v>
       </c>
@@ -1749,8 +1818,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
+    <row r="35" spans="1:5">
+      <c r="A35" s="20"/>
       <c r="C35" t="s">
         <v>49</v>
       </c>
@@ -1758,8 +1827,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+    <row r="36" spans="1:5" ht="15" customHeight="1">
+      <c r="A36" s="19">
         <v>41582</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -1769,8 +1838,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
+    <row r="37" spans="1:5" ht="45">
+      <c r="A37" s="19"/>
       <c r="B37" s="6" t="s">
         <v>62</v>
       </c>
@@ -1781,8 +1850,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
+    <row r="38" spans="1:5">
+      <c r="A38" s="19"/>
       <c r="B38" s="6" t="s">
         <v>64</v>
       </c>
@@ -1793,8 +1862,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
+    <row r="39" spans="1:5">
+      <c r="A39" s="19"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
         <v>154</v>
@@ -1802,9 +1871,12 @@
       <c r="D39" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
+      <c r="E39" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="19"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
         <v>65</v>
@@ -1812,9 +1884,10 @@
       <c r="D40" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
+      <c r="E40" s="28"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="19"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6" t="s">
         <v>170</v>
@@ -1822,9 +1895,12 @@
       <c r="D41" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
+      <c r="E41" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="19"/>
       <c r="B42" s="6" t="s">
         <v>66</v>
       </c>
@@ -1834,9 +1910,10 @@
       <c r="D42" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
+      <c r="E42" s="28"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="19"/>
       <c r="B43" t="s">
         <v>67</v>
       </c>
@@ -1846,18 +1923,24 @@
       <c r="D43" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
+      <c r="E43" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="19"/>
       <c r="C44" t="s">
         <v>69</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
+      <c r="E44" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="19"/>
       <c r="B45" t="s">
         <v>19</v>
       </c>
@@ -1867,18 +1950,20 @@
       <c r="D45" s="8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
+      <c r="E45" s="28"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="19"/>
       <c r="C46" t="s">
         <v>71</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
+      <c r="E46" s="28"/>
+    </row>
+    <row r="47" spans="1:5" ht="75">
+      <c r="A47" s="19"/>
       <c r="B47" t="s">
         <v>62</v>
       </c>
@@ -1888,9 +1973,10 @@
       <c r="D47" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
+      <c r="E47" s="28"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="19"/>
       <c r="B48" t="s">
         <v>19</v>
       </c>
@@ -1900,9 +1986,10 @@
       <c r="D48" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
+      <c r="E48" s="28"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="19"/>
       <c r="B49" t="s">
         <v>74</v>
       </c>
@@ -1912,9 +1999,12 @@
       <c r="D49" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
+      <c r="E49" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="19"/>
       <c r="B50" t="s">
         <v>76</v>
       </c>
@@ -1924,9 +2014,15 @@
       <c r="D50" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
+      <c r="E50" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="F50" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="30">
+      <c r="A51" s="19"/>
       <c r="B51" t="s">
         <v>62</v>
       </c>
@@ -1936,9 +2032,10 @@
       <c r="D51" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
+      <c r="E51" s="28"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="19"/>
       <c r="B52" t="s">
         <v>79</v>
       </c>
@@ -1948,9 +2045,10 @@
       <c r="D52" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
+      <c r="E52" s="28"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="19"/>
       <c r="B53" t="s">
         <v>81</v>
       </c>
@@ -1960,9 +2058,15 @@
       <c r="D53" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
+      <c r="E53" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="F53" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="19"/>
       <c r="B54" t="s">
         <v>83</v>
       </c>
@@ -1972,9 +2076,10 @@
       <c r="D54" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
+      <c r="E54" s="28"/>
+    </row>
+    <row r="55" spans="1:6" ht="60">
+      <c r="A55" s="19"/>
       <c r="B55" t="s">
         <v>62</v>
       </c>
@@ -1984,9 +2089,10 @@
       <c r="D55" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
+      <c r="E55" s="28"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="19"/>
       <c r="B56" t="s">
         <v>62</v>
       </c>
@@ -1996,27 +2102,30 @@
       <c r="D56" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
+      <c r="E56" s="28"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="19"/>
       <c r="C57" t="s">
         <v>86</v>
       </c>
       <c r="D57" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
+      <c r="E57" s="28"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="19"/>
       <c r="C58" t="s">
         <v>87</v>
       </c>
       <c r="D58" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
+      <c r="E58" s="28"/>
+    </row>
+    <row r="59" spans="1:6" ht="75">
+      <c r="A59" s="19"/>
       <c r="B59" t="s">
         <v>62</v>
       </c>
@@ -2026,9 +2135,10 @@
       <c r="D59" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
+      <c r="E59" s="28"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="19"/>
       <c r="B60" t="s">
         <v>90</v>
       </c>
@@ -2038,59 +2148,69 @@
       <c r="D60" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
+      <c r="E60" s="28"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="19"/>
       <c r="C61" t="s">
         <v>98</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="21" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
+      <c r="E61" s="27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="19"/>
       <c r="C62" t="s">
         <v>99</v>
       </c>
-      <c r="D62" s="19"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="17"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="27"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="19"/>
       <c r="C63" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D63" s="19"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="17"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="27"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="19"/>
       <c r="C64" t="s">
         <v>101</v>
       </c>
-      <c r="D64" s="19"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="17"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="27"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="19"/>
       <c r="C65" t="s">
         <v>102</v>
       </c>
-      <c r="D65" s="19"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="17"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="27"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="19"/>
       <c r="C66" t="s">
         <v>103</v>
       </c>
-      <c r="D66" s="19"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="27"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="19"/>
       <c r="B67" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="17"/>
+      <c r="E67" s="28"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="19"/>
       <c r="B68" t="s">
         <v>50</v>
       </c>
@@ -2100,9 +2220,12 @@
       <c r="D68" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
+      <c r="E68" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="19"/>
       <c r="B69" s="3" t="s">
         <v>91</v>
       </c>
@@ -2112,45 +2235,50 @@
       <c r="D69" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
+      <c r="E69" s="28"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="19"/>
       <c r="C70" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D70" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="17"/>
+      <c r="E70" s="28"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="19"/>
       <c r="C71" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D71" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
+      <c r="E71" s="28"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="19"/>
       <c r="C72" s="4" t="s">
         <v>95</v>
       </c>
       <c r="D72" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="17"/>
+      <c r="E72" s="28"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="19"/>
       <c r="C73" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D73" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="17"/>
+      <c r="E73" s="28"/>
+    </row>
+    <row r="74" spans="1:5" ht="45">
+      <c r="A74" s="19"/>
       <c r="B74" t="s">
         <v>62</v>
       </c>
@@ -2160,9 +2288,10 @@
       <c r="D74" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="17"/>
+      <c r="E74" s="28"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="19"/>
       <c r="B75" t="s">
         <v>105</v>
       </c>
@@ -2172,9 +2301,12 @@
       <c r="D75" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="17"/>
+      <c r="E75" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="19"/>
       <c r="B76" t="s">
         <v>107</v>
       </c>
@@ -2184,18 +2316,22 @@
       <c r="D76" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="17"/>
+      <c r="E76" s="28"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="19"/>
       <c r="C77" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="17"/>
+      <c r="E77" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="19"/>
       <c r="B78" t="s">
         <v>110</v>
       </c>
@@ -2205,9 +2341,10 @@
       <c r="D78" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="17"/>
+      <c r="E78" s="28"/>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="19"/>
       <c r="B79" t="s">
         <v>112</v>
       </c>
@@ -2217,9 +2354,10 @@
       <c r="D79" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="17"/>
+      <c r="E79" s="28"/>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="19"/>
       <c r="B80" t="s">
         <v>114</v>
       </c>
@@ -2227,9 +2365,10 @@
         <v>153</v>
       </c>
       <c r="D80" s="8"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="17"/>
+      <c r="E80" s="28"/>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="19"/>
       <c r="B81" t="s">
         <v>115</v>
       </c>
@@ -2239,9 +2378,10 @@
       <c r="D81" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="17">
+      <c r="E81" s="28"/>
+    </row>
+    <row r="82" spans="1:5" ht="15" customHeight="1">
+      <c r="A82" s="19">
         <v>41610</v>
       </c>
       <c r="B82" t="s">
@@ -2253,9 +2393,10 @@
       <c r="D82" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="17"/>
+      <c r="E82" s="28"/>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="19"/>
       <c r="B83" t="s">
         <v>207</v>
       </c>
@@ -2265,45 +2406,55 @@
       <c r="D83" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
-      <c r="B84" t="s">
+      <c r="E83" s="28"/>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="19"/>
+      <c r="B84" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D84" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
-      <c r="B85" t="s">
+      <c r="E84" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="19"/>
+      <c r="B85" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="D85" s="6" t="s">
+      <c r="D85" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="17"/>
-      <c r="B86" t="s">
+      <c r="E85" s="28" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="19"/>
+      <c r="B86" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="24" t="s">
         <v>295</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D86" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="17"/>
+      <c r="E86" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="19"/>
       <c r="B87" t="s">
         <v>74</v>
       </c>
@@ -2313,9 +2464,10 @@
       <c r="D87" s="6" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="17"/>
+      <c r="E87" s="28"/>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="19"/>
       <c r="B88" t="s">
         <v>9</v>
       </c>
@@ -2325,30 +2477,38 @@
       <c r="D88" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="17"/>
-      <c r="B89" t="s">
+      <c r="E88" s="28"/>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="19"/>
+      <c r="B89" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D89" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-      <c r="C90" s="4" t="s">
+      <c r="E89" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="19"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="D90" s="6" t="s">
+      <c r="D90" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="17"/>
+      <c r="E90" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="19"/>
       <c r="B91" t="s">
         <v>66</v>
       </c>
@@ -2358,101 +2518,111 @@
       <c r="D91" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
+      <c r="E91" s="28"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="19"/>
       <c r="C92" s="4" t="s">
         <v>216</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="17"/>
+      <c r="E92" s="28"/>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="19"/>
       <c r="C93" s="4" t="s">
         <v>217</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="17"/>
-      <c r="C94" s="4" t="s">
+      <c r="E93" s="28"/>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="19"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="D94" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="17"/>
+      <c r="E94" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="19"/>
       <c r="B95" t="s">
         <v>218</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D95" s="20" t="s">
+      <c r="D95" s="18" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="17"/>
+    <row r="96" spans="1:5" ht="45">
+      <c r="A96" s="19"/>
       <c r="C96" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="D96" s="20"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="17"/>
+      <c r="D96" s="18"/>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="19"/>
       <c r="C97" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D97" s="20"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
+      <c r="D97" s="18"/>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="19"/>
       <c r="C98" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D98" s="20"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="17"/>
+      <c r="D98" s="18"/>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="19"/>
       <c r="C99" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D99" s="20"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="17"/>
+      <c r="D99" s="18"/>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="19"/>
       <c r="C100" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D100" s="20"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="17"/>
+      <c r="D100" s="18"/>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="19"/>
       <c r="B101" t="s">
         <v>225</v>
       </c>
-      <c r="D101" s="20"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
-      <c r="B102" t="s">
+      <c r="D101" s="18"/>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="19"/>
+      <c r="B102" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="D102" s="23" t="s">
+      <c r="D102" s="25" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" s="15"/>
       <c r="B103" t="s">
         <v>274</v>
@@ -2460,29 +2630,36 @@
       <c r="C103" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D103" s="23" t="s">
+      <c r="D103" s="17" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="28"/>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="15"/>
-      <c r="C104" s="4" t="s">
+      <c r="B104" s="2"/>
+      <c r="C104" s="24" t="s">
         <v>276</v>
       </c>
-      <c r="D104" s="23" t="s">
+      <c r="D104" s="25" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="15"/>
-      <c r="C105" s="4" t="s">
+      <c r="B105" s="2"/>
+      <c r="C105" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="D105" s="23" t="s">
+      <c r="D105" s="25" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="27"/>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="15"/>
       <c r="C106" s="4" t="s">
         <v>278</v>
@@ -2490,17 +2667,22 @@
       <c r="D106" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="28"/>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="15"/>
-      <c r="C107" s="4" t="s">
+      <c r="B107" s="2"/>
+      <c r="C107" s="24" t="s">
         <v>279</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="15"/>
       <c r="B108" t="s">
         <v>280</v>
@@ -2511,8 +2693,9 @@
       <c r="D108" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="28"/>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="15"/>
       <c r="C109" s="4" t="s">
         <v>282</v>
@@ -2520,32 +2703,39 @@
       <c r="D109" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="28"/>
+    </row>
+    <row r="110" spans="1:5" ht="15" customHeight="1">
       <c r="A110" s="15"/>
-      <c r="B110" t="s">
+      <c r="B110" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="29" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="30">
       <c r="A111" s="15"/>
-      <c r="B111" t="s">
+      <c r="B111" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C111" s="16" t="s">
+      <c r="C111" s="26" t="s">
         <v>287</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" s="15"/>
       <c r="B112" t="s">
         <v>288</v>
@@ -2554,96 +2744,115 @@
       <c r="D112" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="9"/>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="15"/>
-      <c r="B113" t="s">
+      <c r="B113" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="C113" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="D113" s="20" t="s">
+      <c r="D113" s="21" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" s="15"/>
-      <c r="C114" s="16" t="s">
+      <c r="B114" s="2"/>
+      <c r="C114" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="D114" s="20"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="21"/>
+      <c r="E114" s="27"/>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="15"/>
-      <c r="C115" s="16" t="s">
+      <c r="B115" s="2"/>
+      <c r="C115" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="D115" s="20"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="21"/>
+      <c r="E115" s="27"/>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="15"/>
-      <c r="C116" s="16" t="s">
+      <c r="B116" s="2"/>
+      <c r="C116" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="D116" s="20"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="21"/>
+      <c r="E116" s="27"/>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="15"/>
-      <c r="C117" s="16" t="s">
+      <c r="B117" s="2"/>
+      <c r="C117" s="26" t="s">
         <v>292</v>
       </c>
-      <c r="D117" s="20"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="21"/>
+      <c r="E117" s="27"/>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="15"/>
-      <c r="C118" s="16" t="s">
+      <c r="B118" s="2"/>
+      <c r="C118" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="D118" s="20"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="21"/>
+      <c r="E118" s="27"/>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="15"/>
-      <c r="C119" s="16" t="s">
+      <c r="B119" s="2"/>
+      <c r="C119" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="D119" s="20"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="21"/>
+      <c r="E119" s="27"/>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="15"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="15"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="15"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="15"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="15"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="15"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="15"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="15"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="15"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1">
       <c r="A129" s="15"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1">
       <c r="A130" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="E61:E66"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="E113:E119"/>
     <mergeCell ref="D113:D119"/>
     <mergeCell ref="A3:A35"/>
     <mergeCell ref="A36:A81"/>
@@ -2653,26 +2862,27 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:D47"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+    <row r="2" spans="1:3" ht="15" customHeight="1">
+      <c r="A2" s="19">
         <v>41582</v>
       </c>
       <c r="B2" t="s">
@@ -2682,14 +2892,14 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+    <row r="3" spans="1:3">
+      <c r="A3" s="19"/>
       <c r="C3" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+    <row r="4" spans="1:3">
+      <c r="A4" s="19"/>
       <c r="B4" t="s">
         <v>57</v>
       </c>
@@ -2697,8 +2907,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+    <row r="5" spans="1:3">
+      <c r="A5" s="19"/>
       <c r="B5" t="s">
         <v>118</v>
       </c>
@@ -2706,8 +2916,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:3">
+      <c r="A6" s="19"/>
       <c r="B6" t="s">
         <v>120</v>
       </c>
@@ -2715,14 +2925,14 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:3">
+      <c r="A7" s="19"/>
       <c r="C7" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+    <row r="8" spans="1:3">
+      <c r="A8" s="19"/>
       <c r="B8" t="s">
         <v>126</v>
       </c>
@@ -2730,8 +2940,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+    <row r="9" spans="1:3">
+      <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>127</v>
       </c>
@@ -2739,8 +2949,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+    <row r="10" spans="1:3">
+      <c r="A10" s="19"/>
       <c r="B10" t="s">
         <v>164</v>
       </c>
@@ -2748,51 +2958,51 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:3">
+      <c r="A11" s="19"/>
       <c r="C11" s="10" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:3" ht="30">
+      <c r="A12" s="19"/>
       <c r="C12" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:3">
+      <c r="A13" s="19"/>
       <c r="C13" s="10" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+    <row r="14" spans="1:3">
+      <c r="A14" s="19"/>
       <c r="B14" t="s">
         <v>126</v>
       </c>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:3">
+      <c r="A15" s="19"/>
       <c r="C15" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:3">
+      <c r="A16" s="19"/>
       <c r="C16" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:4">
+      <c r="A17" s="19"/>
       <c r="C17" s="10" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:4">
+      <c r="A18" s="19"/>
       <c r="B18" t="s">
         <v>165</v>
       </c>
@@ -2800,8 +3010,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+    <row r="19" spans="1:4">
+      <c r="A19" s="22">
         <v>41610</v>
       </c>
       <c r="B19" t="s">
@@ -2814,8 +3024,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+    <row r="20" spans="1:4" ht="30">
+      <c r="A20" s="22"/>
       <c r="C20" s="10" t="s">
         <v>176</v>
       </c>
@@ -2823,8 +3033,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+    <row r="21" spans="1:4">
+      <c r="A21" s="22"/>
       <c r="C21" s="10" t="s">
         <v>175</v>
       </c>
@@ -2832,8 +3042,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
+    <row r="22" spans="1:4" ht="60">
+      <c r="A22" s="22"/>
       <c r="C22" s="3" t="s">
         <v>177</v>
       </c>
@@ -2841,8 +3051,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
+    <row r="23" spans="1:4">
+      <c r="A23" s="22"/>
       <c r="C23" s="10" t="s">
         <v>178</v>
       </c>
@@ -2850,8 +3060,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+    <row r="24" spans="1:4">
+      <c r="A24" s="22"/>
       <c r="C24" s="10" t="s">
         <v>180</v>
       </c>
@@ -2859,8 +3069,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+    <row r="25" spans="1:4" ht="60">
+      <c r="A25" s="22"/>
       <c r="C25" s="10" t="s">
         <v>179</v>
       </c>
@@ -2868,27 +3078,27 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
+    <row r="26" spans="1:4">
+      <c r="A26" s="22"/>
       <c r="B26" t="s">
         <v>182</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="18" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
+    <row r="27" spans="1:4" ht="30">
+      <c r="A27" s="22"/>
       <c r="C27" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="D27" s="20"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
+      <c r="D27" s="18"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="22"/>
       <c r="B28" t="s">
         <v>270</v>
       </c>
@@ -2899,8 +3109,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
+    <row r="29" spans="1:4">
+      <c r="A29" s="22"/>
       <c r="C29" s="3" t="s">
         <v>185</v>
       </c>
@@ -2908,8 +3118,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
+    <row r="30" spans="1:4">
+      <c r="A30" s="22"/>
       <c r="C30" s="3" t="s">
         <v>186</v>
       </c>
@@ -2917,8 +3127,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+    <row r="31" spans="1:4">
+      <c r="A31" s="22"/>
       <c r="B31" t="s">
         <v>193</v>
       </c>
@@ -2929,8 +3139,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+    <row r="32" spans="1:4">
+      <c r="A32" s="22"/>
       <c r="B32" t="s">
         <v>188</v>
       </c>
@@ -2941,8 +3151,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+    <row r="33" spans="1:4">
+      <c r="A33" s="22"/>
       <c r="B33" t="s">
         <v>190</v>
       </c>
@@ -2950,8 +3160,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
+    <row r="34" spans="1:4">
+      <c r="A34" s="22"/>
       <c r="B34" t="s">
         <v>187</v>
       </c>
@@ -2962,19 +3172,19 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+    <row r="35" spans="1:4" ht="30">
+      <c r="A35" s="22"/>
       <c r="C35" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+    <row r="36" spans="1:4">
+      <c r="A36" s="22"/>
       <c r="C36" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="5"/>
       <c r="B37" t="s">
         <v>164</v>
@@ -2983,18 +3193,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="30">
       <c r="A38" s="5"/>
       <c r="C38" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="C39" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="B40" t="s">
         <v>126</v>
       </c>
@@ -3002,17 +3212,17 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="C41" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="C42" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="B43" t="s">
         <v>199</v>
       </c>
@@ -3020,22 +3230,22 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="C44" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="30">
       <c r="C45" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="B46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="B47" t="s">
         <v>204</v>
       </c>
@@ -3051,22 +3261,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+    <row r="2" spans="1:3">
+      <c r="A2" s="19">
         <v>41582</v>
       </c>
       <c r="B2" t="s">
@@ -3076,20 +3286,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+    <row r="3" spans="1:3">
+      <c r="A3" s="19"/>
       <c r="C3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+    <row r="4" spans="1:3">
+      <c r="A4" s="19"/>
       <c r="C4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+    <row r="5" spans="1:3">
+      <c r="A5" s="19"/>
       <c r="B5" t="s">
         <v>132</v>
       </c>
@@ -3097,8 +3307,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:3">
+      <c r="A6" s="19"/>
       <c r="B6" t="s">
         <v>134</v>
       </c>
@@ -3106,17 +3316,17 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:3">
+      <c r="A7" s="19"/>
       <c r="C7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+    <row r="8" spans="1:3">
+      <c r="A8" s="19"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3127,73 +3337,73 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+    <row r="2" spans="1:3" ht="15" customHeight="1">
+      <c r="A2" s="19">
         <v>41582</v>
       </c>
       <c r="B2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+    <row r="3" spans="1:3">
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+    <row r="4" spans="1:3">
+      <c r="A4" s="19"/>
       <c r="B4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+    <row r="5" spans="1:3">
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:3">
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:3">
+      <c r="A7" s="19"/>
       <c r="B7" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+    <row r="8" spans="1:3">
+      <c r="A8" s="19"/>
       <c r="B8" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+    <row r="9" spans="1:3">
+      <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+    <row r="10" spans="1:3">
+      <c r="A10" s="19"/>
       <c r="B10" s="1" t="s">
         <v>145</v>
       </c>
@@ -3201,8 +3411,8 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:3">
+      <c r="A11" s="19"/>
       <c r="B11" s="1" t="s">
         <v>146</v>
       </c>
@@ -3210,8 +3420,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:3">
+      <c r="A12" s="19"/>
       <c r="B12" s="1" t="s">
         <v>147</v>
       </c>
@@ -3219,8 +3429,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:3">
+      <c r="A13" s="19"/>
       <c r="B13" s="1" t="s">
         <v>148</v>
       </c>
@@ -3237,37 +3447,37 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="67.85546875" customWidth="1"/>
     <col min="4" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="13"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+    <row r="2" spans="1:7">
+      <c r="A2" s="19">
         <v>41600</v>
       </c>
       <c r="B2" t="s">
@@ -3280,8 +3490,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+    <row r="3" spans="1:7">
+      <c r="A3" s="19"/>
       <c r="B3" t="s">
         <v>228</v>
       </c>
@@ -3292,20 +3502,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+    <row r="4" spans="1:7">
+      <c r="A4" s="19"/>
       <c r="C4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+    <row r="5" spans="1:7">
+      <c r="A5" s="19"/>
       <c r="C5" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:7">
+      <c r="A6" s="19"/>
       <c r="B6" t="s">
         <v>230</v>
       </c>
@@ -3316,8 +3526,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:7">
+      <c r="A7" s="19"/>
       <c r="B7" t="s">
         <v>232</v>
       </c>
@@ -3328,8 +3538,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+    <row r="8" spans="1:7">
+      <c r="A8" s="19"/>
       <c r="C8" t="s">
         <v>266</v>
       </c>
@@ -3337,14 +3547,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+    <row r="9" spans="1:7">
+      <c r="A9" s="19"/>
       <c r="C9" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+    <row r="10" spans="1:7">
+      <c r="A10" s="19"/>
       <c r="B10" t="s">
         <v>234</v>
       </c>
@@ -3355,8 +3565,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:7">
+      <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>236</v>
       </c>
@@ -3364,8 +3574,8 @@
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:7">
+      <c r="A12" s="19"/>
       <c r="B12" t="s">
         <v>236</v>
       </c>
@@ -3373,11 +3583,11 @@
         <v>238</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="19"/>
       <c r="B14" t="s">
         <v>247</v>
       </c>
@@ -3397,38 +3607,38 @@
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19"/>
       <c r="C15" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="C16" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="C17" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="C18" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="C19" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="C20" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" t="s">
         <v>248</v>
       </c>
@@ -3442,59 +3652,59 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="C23" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" t="s">
         <v>253</v>
       </c>
       <c r="C25" t="s">
         <v>254</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="23" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="C26" t="s">
         <v>255</v>
       </c>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="23"/>
+    </row>
+    <row r="27" spans="2:5">
       <c r="C27" t="s">
         <v>256</v>
       </c>
-      <c r="D27" s="22"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="23"/>
+    </row>
+    <row r="28" spans="2:5">
       <c r="C28" t="s">
         <v>257</v>
       </c>
-      <c r="D28" s="22"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="23"/>
+    </row>
+    <row r="29" spans="2:5">
       <c r="C29" t="s">
         <v>258</v>
       </c>
-      <c r="D29" s="22"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="23"/>
+    </row>
+    <row r="30" spans="2:5">
       <c r="C30" t="s">
         <v>259</v>
       </c>
-      <c r="D30" s="22"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="23"/>
+    </row>
+    <row r="31" spans="2:5">
       <c r="C31" t="s">
         <v>260</v>
       </c>
-      <c r="D31" s="22"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="23"/>
+    </row>
+    <row r="32" spans="2:5">
       <c r="B32" t="s">
         <v>261</v>
       </c>

</xml_diff>